<commit_message>
backend: Game compelete rest endpoint
</commit_message>
<xml_diff>
--- a/hours.xlsx
+++ b/hours.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niko/Documents/dev_projects/kt-tournament/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4315294-7512-2648-8D37-1254ECBEC9BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E574A18-9CDD-6944-B01E-2A9EFC050F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{F639157B-5556-604D-B26D-3FE90CE32124}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Creating the directory and installing proper tools. Created also a simple player RESTful repository.</t>
   </si>
@@ -57,6 +57,15 @@
   </si>
   <si>
     <t>Used hours</t>
+  </si>
+  <si>
+    <t>Backend object classes, REST endpoints</t>
+  </si>
+  <si>
+    <t>Backend object model assember, ThunderClient testing</t>
+  </si>
+  <si>
+    <t>Backend test dataLoader thinkering</t>
   </si>
 </sst>
 </file>
@@ -475,7 +484,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,7 +522,7 @@
       </c>
       <c r="H3">
         <f>SUM(C4:C20)</f>
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
@@ -528,19 +537,37 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="2">
+        <v>45441</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="B6" s="2">
+        <v>45442</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="B7" s="2">
+        <v>45443</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="1"/>

</xml_diff>